<commit_message>
Update Test Plan, Improve Logging, Improve Tests, Improve TME1 Functionality
</commit_message>
<xml_diff>
--- a/course-work/COMP308TestPlans.xlsx
+++ b/course-work/COMP308TestPlans.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Circles" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="98">
   <si>
     <t>Test ID</t>
   </si>
@@ -78,6 +78,261 @@
   </si>
   <si>
     <t>Circles</t>
+  </si>
+  <si>
+    <t>Circle</t>
+  </si>
+  <si>
+    <t>(Constructor)</t>
+  </si>
+  <si>
+    <t>Initialization - No Params</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Initialization - Params within range</t>
+  </si>
+  <si>
+    <t>Creates circle with supplied values</t>
+  </si>
+  <si>
+    <t>As Expected</t>
+  </si>
+  <si>
+    <t>Initialization - Params over radius range</t>
+  </si>
+  <si>
+    <t>Creates circle with supplied values and max radius</t>
+  </si>
+  <si>
+    <t>Initialization - Params negative ranges</t>
+  </si>
+  <si>
+    <t>double 10 
+double 10
+double 200</t>
+  </si>
+  <si>
+    <t>double 10
+double 10
+double 5</t>
+  </si>
+  <si>
+    <t>double -45
+double -30
+double -300</t>
+  </si>
+  <si>
+    <t>Creates circle with supplied values and max radius with negative numbers</t>
+  </si>
+  <si>
+    <t>Calculate circumference of supplied Circle from TestID=2</t>
+  </si>
+  <si>
+    <t>Calculate area of default Circle object</t>
+  </si>
+  <si>
+    <t>Calculate circumference of default Circle object</t>
+  </si>
+  <si>
+    <t>Calculate area of Circle object from TestID=2</t>
+  </si>
+  <si>
+    <t>circumference</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>setRadius</t>
+  </si>
+  <si>
+    <t>Set radius with a float value</t>
+  </si>
+  <si>
+    <t>Exception: Invalid argument</t>
+  </si>
+  <si>
+    <t>double 5.6</t>
+  </si>
+  <si>
+    <t>Set radius with out of range value</t>
+  </si>
+  <si>
+    <t>double 400</t>
+  </si>
+  <si>
+    <t>Set's the radius to MAX_RADIUS= 10</t>
+  </si>
+  <si>
+    <t>Set radius within range value</t>
+  </si>
+  <si>
+    <t>double 8</t>
+  </si>
+  <si>
+    <t>Set's the radius=8</t>
+  </si>
+  <si>
+    <t>printAttributes</t>
+  </si>
+  <si>
+    <t>Prints the coordinates of default Circle</t>
+  </si>
+  <si>
+    <t>Prints the default values of a Circle</t>
+  </si>
+  <si>
+    <t>Prints the coordinates of Circle from TestID=2</t>
+  </si>
+  <si>
+    <t>isInside</t>
+  </si>
+  <si>
+    <t>Checks a point which is inside default Circle</t>
+  </si>
+  <si>
+    <t>Create default Circle object with default values x=10, y=10, radius=5</t>
+  </si>
+  <si>
+    <t>T1P1-1</t>
+  </si>
+  <si>
+    <t>T1P1-2</t>
+  </si>
+  <si>
+    <t>T1P1-3</t>
+  </si>
+  <si>
+    <t>T1P1-4</t>
+  </si>
+  <si>
+    <t>T1P1-5</t>
+  </si>
+  <si>
+    <t>T1P1-6</t>
+  </si>
+  <si>
+    <t>T1P1-7</t>
+  </si>
+  <si>
+    <t>T1P1-8</t>
+  </si>
+  <si>
+    <t>T1P1-9</t>
+  </si>
+  <si>
+    <t>T1P1-10</t>
+  </si>
+  <si>
+    <t>T1P1-11</t>
+  </si>
+  <si>
+    <t>T1P1-12</t>
+  </si>
+  <si>
+    <t>T1P1-13</t>
+  </si>
+  <si>
+    <t>T1P1-14</t>
+  </si>
+  <si>
+    <t>T1P1-15</t>
+  </si>
+  <si>
+    <t>T1P1-16</t>
+  </si>
+  <si>
+    <t>T1P1-17</t>
+  </si>
+  <si>
+    <t>T1P1-18</t>
+  </si>
+  <si>
+    <t>T1P1-19</t>
+  </si>
+  <si>
+    <t>Prints the values of Circle from TestID=T1P1-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate area of default TestID=T1P1-1 Circle = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate area of TestID=T1P1-2 Circle = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate circumference of  TestID=T1P1-2 Circle = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate circumference of TestID=T1P1-1 default Circle = </t>
+  </si>
+  <si>
+    <t>move</t>
+  </si>
+  <si>
+    <t>Checks a point which is out default Circle</t>
+  </si>
+  <si>
+    <t>Check a point directly on the edge of a Circle</t>
+  </si>
+  <si>
+    <t>double 3
+double 2</t>
+  </si>
+  <si>
+    <t>double 80
+double -80</t>
+  </si>
+  <si>
+    <t>double 10
+double 10</t>
+  </si>
+  <si>
+    <t>Returns true</t>
+  </si>
+  <si>
+    <t>Returns false</t>
+  </si>
+  <si>
+    <t>returns false</t>
+  </si>
+  <si>
+    <t>Increase the Circles center point location</t>
+  </si>
+  <si>
+    <t>Decrease the Circles center point location</t>
+  </si>
+  <si>
+    <t>double 2
+double 4</t>
+  </si>
+  <si>
+    <t>double -20
+double -40</t>
+  </si>
+  <si>
+    <t>double 1.79769313486231570e+308d
+double -1.79769313486231570e+308d</t>
+  </si>
+  <si>
+    <t>Increase/ Decrease the Circle's center point by the max capacity of a double value</t>
+  </si>
+  <si>
+    <t>Moves the Circle's center point to new increased location</t>
+  </si>
+  <si>
+    <t>Moves the Circle's center point to new decreased location</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Moves the Circle's center point to new increased/ decreased location</t>
   </si>
 </sst>
 </file>
@@ -85,7 +340,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -119,12 +374,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -250,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -299,10 +560,6 @@
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -311,11 +568,168 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-4.9989318521683403E-2"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -866,159 +1280,6 @@
         <bottom style="medium">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="0" tint="-4.9989318521683403E-2"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1070,64 +1331,64 @@
   <autoFilter ref="A5:H24"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Test ID" dataDxfId="34"/>
-    <tableColumn id="2" name="Class" dataDxfId="33"/>
-    <tableColumn id="3" name="Method" dataDxfId="32"/>
-    <tableColumn id="4" name="Description" dataDxfId="31"/>
-    <tableColumn id="5" name="Input" dataDxfId="30"/>
-    <tableColumn id="6" name="Expected Result" dataDxfId="29"/>
-    <tableColumn id="7" name="Actual Result" dataDxfId="28"/>
-    <tableColumn id="8" name="01-Oct-14" dataDxfId="27"/>
+    <tableColumn id="2" name="Class" dataDxfId="6"/>
+    <tableColumn id="3" name="Method" dataDxfId="5"/>
+    <tableColumn id="4" name="Description" dataDxfId="4"/>
+    <tableColumn id="5" name="Input" dataDxfId="3"/>
+    <tableColumn id="6" name="Expected Result" dataDxfId="2"/>
+    <tableColumn id="7" name="Actual Result" dataDxfId="0"/>
+    <tableColumn id="8" name="01-Oct-14" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A5:H24" totalsRowShown="0" tableBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A5:H24" totalsRowShown="0" tableBorderDxfId="33">
   <autoFilter ref="A5:H24"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Test ID" dataDxfId="25"/>
-    <tableColumn id="2" name="Class" dataDxfId="24"/>
-    <tableColumn id="3" name="Method" dataDxfId="23"/>
-    <tableColumn id="4" name="Description" dataDxfId="22"/>
-    <tableColumn id="5" name="Input" dataDxfId="21"/>
-    <tableColumn id="6" name="Expected Result" dataDxfId="20"/>
-    <tableColumn id="7" name="Actual Result" dataDxfId="19"/>
-    <tableColumn id="8" name="01-Oct-14" dataDxfId="18"/>
+    <tableColumn id="1" name="Test ID" dataDxfId="32"/>
+    <tableColumn id="2" name="Class" dataDxfId="31"/>
+    <tableColumn id="3" name="Method" dataDxfId="30"/>
+    <tableColumn id="4" name="Description" dataDxfId="29"/>
+    <tableColumn id="5" name="Input" dataDxfId="28"/>
+    <tableColumn id="6" name="Expected Result" dataDxfId="27"/>
+    <tableColumn id="7" name="Actual Result" dataDxfId="26"/>
+    <tableColumn id="8" name="01-Oct-14" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="A5:H24" totalsRowShown="0" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="A5:H24" totalsRowShown="0" tableBorderDxfId="24">
   <autoFilter ref="A5:H24"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Test ID" dataDxfId="16"/>
-    <tableColumn id="2" name="Class" dataDxfId="15"/>
-    <tableColumn id="3" name="Method" dataDxfId="14"/>
-    <tableColumn id="4" name="Description" dataDxfId="13"/>
-    <tableColumn id="5" name="Input" dataDxfId="12"/>
-    <tableColumn id="6" name="Expected Result" dataDxfId="11"/>
-    <tableColumn id="7" name="Actual Result" dataDxfId="10"/>
-    <tableColumn id="8" name="01-Oct-14" dataDxfId="9"/>
+    <tableColumn id="1" name="Test ID" dataDxfId="23"/>
+    <tableColumn id="2" name="Class" dataDxfId="22"/>
+    <tableColumn id="3" name="Method" dataDxfId="21"/>
+    <tableColumn id="4" name="Description" dataDxfId="20"/>
+    <tableColumn id="5" name="Input" dataDxfId="19"/>
+    <tableColumn id="6" name="Expected Result" dataDxfId="18"/>
+    <tableColumn id="7" name="Actual Result" dataDxfId="17"/>
+    <tableColumn id="8" name="01-Oct-14" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2456" displayName="Table2456" ref="A5:H24" totalsRowShown="0" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table2456" displayName="Table2456" ref="A5:H24" totalsRowShown="0" tableBorderDxfId="15">
   <autoFilter ref="A5:H24"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Test ID" dataDxfId="7"/>
-    <tableColumn id="2" name="Class" dataDxfId="6"/>
-    <tableColumn id="3" name="Method" dataDxfId="5"/>
-    <tableColumn id="4" name="Description" dataDxfId="4"/>
-    <tableColumn id="5" name="Input" dataDxfId="3"/>
-    <tableColumn id="6" name="Expected Result" dataDxfId="2"/>
-    <tableColumn id="7" name="Actual Result" dataDxfId="1"/>
-    <tableColumn id="8" name="01-Oct-14" dataDxfId="0"/>
+    <tableColumn id="1" name="Test ID" dataDxfId="14"/>
+    <tableColumn id="2" name="Class" dataDxfId="13"/>
+    <tableColumn id="3" name="Method" dataDxfId="12"/>
+    <tableColumn id="4" name="Description" dataDxfId="11"/>
+    <tableColumn id="5" name="Input" dataDxfId="10"/>
+    <tableColumn id="6" name="Expected Result" dataDxfId="9"/>
+    <tableColumn id="7" name="Actual Result" dataDxfId="8"/>
+    <tableColumn id="8" name="01-Oct-14" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1398,16 +1659,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="14" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="35.28515625" style="3" customWidth="1"/>
-    <col min="6" max="7" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1427,10 +1691,10 @@
         <v>16</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="G2" s="22">
+      <c r="G2" s="26">
         <v>41898</v>
       </c>
-      <c r="H2" s="23"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
@@ -1441,258 +1705,462 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
-        <v>2</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
-        <v>3</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
-        <v>4</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
-        <v>5</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
-        <v>6</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
-        <v>7</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="10"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
-        <v>8</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="10"/>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="32"/>
+      <c r="H9" s="34"/>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="35"/>
+      <c r="H10" s="34"/>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="32"/>
+      <c r="H11" s="34"/>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="35"/>
+      <c r="H12" s="34"/>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="32"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
-        <v>9</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
-        <v>10</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="10"/>
+      <c r="A14" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="35"/>
+      <c r="H14" s="34"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="32"/>
+      <c r="H15" s="34"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
-        <v>11</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
-        <v>12</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
-        <v>13</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="10"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="16">
-        <v>14</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="10"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
-        <v>15</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="10"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
-        <v>16</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="16">
+      <c r="A16" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
-        <v>18</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="10"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
-        <v>19</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="13"/>
+      <c r="C16" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="35"/>
+      <c r="H16" s="34"/>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="32"/>
+      <c r="H17" s="34"/>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="35"/>
+      <c r="H18" s="34"/>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="32"/>
+      <c r="H19" s="34"/>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="35"/>
+      <c r="H20" s="34"/>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="32"/>
+      <c r="H21" s="34"/>
+    </row>
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" s="32"/>
+      <c r="H22" s="34"/>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="32"/>
+      <c r="H23" s="34"/>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="32"/>
+      <c r="H24" s="34" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1739,10 +2207,10 @@
         <v>15</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="G2" s="22">
+      <c r="G2" s="26">
         <v>41898</v>
       </c>
-      <c r="H2" s="23"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
@@ -1753,28 +2221,28 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2051,10 +2519,10 @@
         <v>13</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="G2" s="22">
+      <c r="G2" s="26">
         <v>41898</v>
       </c>
-      <c r="H2" s="23"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
@@ -2065,28 +2533,28 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="25" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2334,7 +2802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -2363,10 +2831,10 @@
         <v>12</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="G2" s="22">
+      <c r="G2" s="26">
         <v>41898</v>
       </c>
-      <c r="H2" s="23"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
@@ -2377,28 +2845,28 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="25" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>